<commit_message>
adjusted some formats and add one figure in casestudy.tex
</commit_message>
<xml_diff>
--- a/other/CaseStudy.xlsx
+++ b/other/CaseStudy.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
   <si>
     <t>Normalized Energy</t>
   </si>
@@ -61,6 +62,12 @@
   </si>
   <si>
     <t>Energy opt.</t>
+  </si>
+  <si>
+    <t>read probability</t>
+  </si>
+  <si>
+    <t>write probability</t>
   </si>
 </sst>
 </file>
@@ -123,10 +130,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526426"/>
-          <c:y val="0.11449276309341"/>
-          <c:w val="0.82772481120027253"/>
-          <c:h val="0.60071966107970942"/>
+          <c:x val="0.13494304021526429"/>
+          <c:y val="0.11449276309341001"/>
+          <c:w val="0.82772481120027275"/>
+          <c:h val="0.60071966107970953"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -405,26 +412,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="50315648"/>
-        <c:axId val="50348800"/>
+        <c:axId val="99829248"/>
+        <c:axId val="99830784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50315648"/>
+        <c:axId val="99829248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50348800"/>
+        <c:crossAx val="99830784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50348800"/>
+        <c:axId val="99830784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,7 +456,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50315648"/>
+        <c:crossAx val="99829248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -462,9 +468,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.18018060737653438"/>
-          <c:y val="5.8550373511004697E-4"/>
-          <c:w val="0.63560110640321454"/>
-          <c:h val="9.906172567589891E-2"/>
+          <c:y val="5.8550373511004707E-4"/>
+          <c:w val="0.63560110640321477"/>
+          <c:h val="9.9061725675898937E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -482,7 +488,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -500,10 +506,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526432"/>
-          <c:y val="0.11449276309341003"/>
-          <c:w val="0.82772481120027286"/>
-          <c:h val="0.5867957294811833"/>
+          <c:x val="0.13494304021526438"/>
+          <c:y val="0.11449276309341004"/>
+          <c:w val="0.82772481120027308"/>
+          <c:h val="0.58679572948118341"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -782,25 +788,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="132283392"/>
-        <c:axId val="144163584"/>
+        <c:axId val="100143488"/>
+        <c:axId val="100145024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132283392"/>
+        <c:axId val="100143488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144163584"/>
+        <c:crossAx val="100145024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144163584"/>
+        <c:axId val="100145024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +832,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132283392"/>
+        <c:crossAx val="100143488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -839,8 +845,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.18018060737653438"/>
           <c:y val="5.8550373511004707E-4"/>
-          <c:w val="0.63560110640321499"/>
-          <c:h val="9.9061725675898965E-2"/>
+          <c:w val="0.63560110640321521"/>
+          <c:h val="9.9061725675898979E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -858,7 +864,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -876,10 +882,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526443"/>
-          <c:y val="0.11449276309341005"/>
-          <c:w val="0.8277248112002733"/>
-          <c:h val="0.58679572948118353"/>
+          <c:x val="0.13494304021526446"/>
+          <c:y val="0.11449276309341007"/>
+          <c:w val="0.82772481120027352"/>
+          <c:h val="0.58679572948118364"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1158,25 +1164,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="52257536"/>
-        <c:axId val="53875072"/>
+        <c:axId val="100174848"/>
+        <c:axId val="100180736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52257536"/>
+        <c:axId val="100174848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53875072"/>
+        <c:crossAx val="100180736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53875072"/>
+        <c:axId val="100180736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,7 +1208,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52257536"/>
+        <c:crossAx val="100174848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1215,8 +1221,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.18018060737653438"/>
           <c:y val="5.8550373511004707E-4"/>
-          <c:w val="0.63560110640321543"/>
-          <c:h val="9.9061725675899007E-2"/>
+          <c:w val="0.63560110640321565"/>
+          <c:h val="9.9061725675899034E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1234,7 +1240,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1252,10 +1258,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526432"/>
-          <c:y val="0.11449276309341003"/>
-          <c:w val="0.82772481120027286"/>
-          <c:h val="0.49125177379910029"/>
+          <c:x val="0.13494304021526438"/>
+          <c:y val="0.11449276309341004"/>
+          <c:w val="0.82772481120027308"/>
+          <c:h val="0.4912517737991004"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1534,11 +1540,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="152489984"/>
-        <c:axId val="152491520"/>
+        <c:axId val="100604160"/>
+        <c:axId val="100618240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152489984"/>
+        <c:axId val="100604160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,14 +1561,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152491520"/>
+        <c:crossAx val="100618240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152491520"/>
+        <c:axId val="100618240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,7 +1594,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152489984"/>
+        <c:crossAx val="100604160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,7 +1607,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.18018060737653438"/>
           <c:y val="5.8550373511004707E-4"/>
-          <c:w val="0.64452966816647916"/>
+          <c:w val="0.64452966816647939"/>
           <c:h val="0.1233043017922862"/>
         </c:manualLayout>
       </c:layout>
@@ -1626,7 +1632,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1644,10 +1650,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526443"/>
-          <c:y val="0.11449276309341005"/>
-          <c:w val="0.8277248112002733"/>
-          <c:h val="0.51611848518935133"/>
+          <c:x val="0.13494304021526446"/>
+          <c:y val="0.11449276309341007"/>
+          <c:w val="0.82772481120027352"/>
+          <c:h val="0.51611848518935122"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1926,25 +1932,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="145189504"/>
-        <c:axId val="145199488"/>
+        <c:axId val="100648064"/>
+        <c:axId val="100649600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145189504"/>
+        <c:axId val="100648064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145199488"/>
+        <c:crossAx val="100649600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145199488"/>
+        <c:axId val="100649600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1971,7 +1977,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145189504"/>
+        <c:crossAx val="100648064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1984,8 +1990,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.18018060737653438"/>
           <c:y val="5.8550373511004707E-4"/>
-          <c:w val="0.63857728721409823"/>
-          <c:h val="0.11430011248593926"/>
+          <c:w val="0.63857728721409834"/>
+          <c:h val="0.11430011248593927"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2009,7 +2015,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2027,10 +2033,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13494304021526449"/>
-          <c:y val="0.15548013413770109"/>
-          <c:w val="0.82772481120027375"/>
-          <c:h val="0.43756776569370581"/>
+          <c:x val="0.13494304021526451"/>
+          <c:y val="0.15548013413770115"/>
+          <c:w val="0.82772481120027386"/>
+          <c:h val="0.43756776569370587"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2309,25 +2315,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="145225216"/>
-        <c:axId val="145226752"/>
+        <c:axId val="100687872"/>
+        <c:axId val="100689408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145225216"/>
+        <c:axId val="100687872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145226752"/>
+        <c:crossAx val="100689408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145226752"/>
+        <c:axId val="100689408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,7 +2359,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145225216"/>
+        <c:crossAx val="100687872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2367,7 +2373,7 @@
           <c:x val="0.18018060737653438"/>
           <c:y val="5.8550373511004707E-4"/>
           <c:w val="0.64750585864266963"/>
-          <c:h val="0.12245345271965294"/>
+          <c:h val="0.12245345271965295"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2391,7 +2397,541 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1502187226596671E-2"/>
+          <c:y val="0.18760731521463042"/>
+          <c:w val="0.87443086855522356"/>
+          <c:h val="0.42335424173673208"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>read probability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$6:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FFT4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FFT512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>math</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mp3enc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mpeg4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsort</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>rj_enc</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>rj_dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$6:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>write probability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$6:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FFT4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FFT512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>math</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mp3enc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mpeg4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsort</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>rj_enc</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>rj_dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$6:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.18999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18999999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="86964864"/>
+        <c:axId val="118948224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="86964864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118948224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="118948224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86964864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20395975503062116"/>
+          <c:y val="4.2457713619130973E-3"/>
+          <c:w val="0.61005987154831454"/>
+          <c:h val="0.19443992887985775"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1502187226596671E-2"/>
+          <c:y val="0.18760731521463042"/>
+          <c:w val="0.87443086855522367"/>
+          <c:h val="0.42335424173673208"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>read probability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$6:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FFT4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FFT512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>math</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mp3enc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mpeg4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsort</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>rj_enc</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>rj_dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$6:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>write probability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$6:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dijkstra</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FFT4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FFT512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>math</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mp3enc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mpeg4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qsort</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>rj_enc</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>rj_dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$6:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.18999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18999999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="133289856"/>
+        <c:axId val="133291392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="133289856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133291392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133291392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133289856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20395975503062122"/>
+          <c:y val="4.2457713619130991E-3"/>
+          <c:w val="0.61005987154831498"/>
+          <c:h val="0.19443992887985775"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2579,6 +3119,76 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2874,8 +3484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:S41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32:H41"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3544,7 +4154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -3557,12 +4167,150 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C5:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:5">
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5">
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.85</v>
+      </c>
+      <c r="E6">
+        <f>1-D6</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5">
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0.54</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E14" si="0">1-D7</f>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5">
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0.54</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5">
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.43999999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5">
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>0.61</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5">
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0.53</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5">
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>0.81</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.18999999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5">
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>0.81</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.18999999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>